<commit_message>
lxml error patch 1.0
</commit_message>
<xml_diff>
--- a/Ali.xlsx
+++ b/Ali.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,10 +536,8 @@
           <t>Frequency distribution and association of Fat-mass and obesity (FTO) gene SNP rs-9939609 variant with Diabetes Mellitus Type-II population of Hyderabad, Sindh, Pakistan</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2021</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -592,6 +590,97 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sam Hodgson</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Genetic basis of early onset and progression of type 2 diabetes in South Asians</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Nature medicine</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PMID: 39592779
+DOI: 10.1038/s41591-024-03317-8</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cohort</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Pakistan</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>11678</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>WES</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Parsed heuristically from abstract/meta.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Parsed heuristically from abstract/meta.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>